<commit_message>
Completed basic structure UwU
</commit_message>
<xml_diff>
--- a/CandidatesData.xlsx
+++ b/CandidatesData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rsrko\Documents\UiPath\Assignment Bolt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C9F24B-DC12-4DF4-BE25-74346A3D224E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48616D26-9533-4BC5-A6EA-6C556BC57CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1344" windowWidth="11040" windowHeight="5676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
     <t>Software Test Engineer(intern)</t>
   </si>
   <si>
-    <t>YES</t>
+    <t>To be checked</t>
   </si>
   <si>
     <t>linkedin.com/in/ashfaaq-eathally-92035b186/</t>
@@ -111,7 +111,7 @@
     <t>linkedin.com/in/alisha-toolsy-4817a722a/</t>
   </si>
   <si>
-    <t>NO</t>
+    <t>Good</t>
   </si>
   <si>
     <t>linkedin.com/in/amanda-dieudonné-b71b03176/</t>
@@ -435,7 +435,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>

</xml_diff>